<commit_message>
Update order registration template with styling and header changes
Add exceljs dependency to package.json and update order_registration_template.xlsx to include yellow background on the second row and change the header of column I.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 5a0337d7-6aeb-4b5d-8c8c-856c59d84f9d
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 151b549b-6e84-45f4-b39a-f86d8fb8623d
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/ffb4be9c-afff-4c4d-909c-bc946915535e/5a0337d7-6aeb-4b5d-8c8c-856c59d84f9d/BvAK3f1
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/public/templates/order_registration_template.xlsx
+++ b/public/templates/order_registration_template.xlsx
@@ -1,55 +1,92 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="주문등록-양식파일" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="주문등록-양식파일" state="visible" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+  <si>
+    <t>주문자명</t>
+  </si>
+  <si>
+    <t>주문자 전화번호</t>
+  </si>
+  <si>
+    <t>주문자 주소</t>
+  </si>
+  <si>
+    <t>수령자명</t>
+  </si>
+  <si>
+    <t>수령자휴대폰번호</t>
+  </si>
+  <si>
+    <t>수령자 전화번호</t>
+  </si>
+  <si>
+    <t>수령자 주소</t>
+  </si>
+  <si>
+    <t>배송메시지</t>
+  </si>
+  <si>
+    <t>상품코드</t>
+  </si>
+  <si>
+    <t>상품명</t>
+  </si>
+  <si>
+    <t>자체주문번호</t>
+  </si>
+  <si>
+    <t>필수</t>
+  </si>
+  <si>
+    <t>선택</t>
+  </si>
+  <si>
+    <t>필수(중복x)</t>
+  </si>
+  <si>
+    <t>→</t>
+  </si>
+  <si>
+    <t xml:space="preserve">이 설명 부분 _x000d_
+은 삭제 후 _x000d_
+작성해 주세요.</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -64,14 +101,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,94 +442,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
+  <sheetFormatPr customHeight="1"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>주문자명</v>
-      </c>
-      <c r="B1" t="str">
-        <v>주문자 전화번호</v>
-      </c>
-      <c r="C1" t="str">
-        <v>주문자 주소</v>
-      </c>
-      <c r="D1" t="str">
-        <v>수령자명</v>
-      </c>
-      <c r="E1" t="str">
-        <v>수령자휴대폰번호</v>
-      </c>
-      <c r="F1" t="str">
-        <v>수령자 전화번호</v>
-      </c>
-      <c r="G1" t="str">
-        <v>수령자 주소</v>
-      </c>
-      <c r="H1" t="str">
-        <v>배송메시지</v>
-      </c>
-      <c r="I1" t="str">
-        <v>상품코드</v>
-      </c>
-      <c r="J1" t="str">
-        <v>상품명</v>
-      </c>
-      <c r="K1" t="str">
-        <v>자체주문번호</v>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" xml:space="preserve">
-      <c r="A2" t="str">
-        <v>필수</v>
-      </c>
-      <c r="B2" t="str">
-        <v>필수</v>
-      </c>
-      <c r="C2" t="str">
-        <v>선택</v>
-      </c>
-      <c r="D2" t="str">
-        <v>필수</v>
-      </c>
-      <c r="E2" t="str">
-        <v>필수</v>
-      </c>
-      <c r="F2" t="str">
-        <v>선택</v>
-      </c>
-      <c r="G2" t="str">
-        <v>필수</v>
-      </c>
-      <c r="H2" t="str">
-        <v>선택</v>
-      </c>
-      <c r="I2" t="str">
-        <v>필수</v>
-      </c>
-      <c r="J2" t="str">
-        <v>필수</v>
-      </c>
-      <c r="K2" t="str">
-        <v>필수(중복x)</v>
-      </c>
-      <c r="L2" t="str">
-        <v>→</v>
-      </c>
-      <c r="M2" t="str" xml:space="preserve">
-        <v xml:space="preserve">이 설명 부분 _x000d_
-은 삭제 후 _x000d_
-작성해 주세요.</v>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M2"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the order registration template with styling and formatting
Recreate and reformat the order registration template (xlsx) with updated styling, including blue header background, bold white text, yellow description row, and corrected column order.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 5a0337d7-6aeb-4b5d-8c8c-856c59d84f9d
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 85785a51-e499-4608-abc0-cd695ce28aaf
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/ffb4be9c-afff-4c4d-909c-bc946915535e/5a0337d7-6aeb-4b5d-8c8c-856c59d84f9d/BvAK3f1
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/public/templates/order_registration_template.xlsx
+++ b/public/templates/order_registration_template.xlsx
@@ -4,22 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="주문등록-양식파일" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="주문등록" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+  <si>
+    <t>자체주문번호</t>
+  </si>
   <si>
     <t>주문자명</t>
   </si>
   <si>
-    <t>주문자 전화번호</t>
-  </si>
-  <si>
-    <t>주문자 주소</t>
+    <t>주문자전화번호</t>
   </si>
   <si>
     <t>수령자명</t>
@@ -28,10 +28,10 @@
     <t>수령자휴대폰번호</t>
   </si>
   <si>
-    <t>수령자 전화번호</t>
-  </si>
-  <si>
-    <t>수령자 주소</t>
+    <t>우편번호</t>
+  </si>
+  <si>
+    <t>수령자주소</t>
   </si>
   <si>
     <t>배송메시지</t>
@@ -43,31 +43,47 @@
     <t>상품명</t>
   </si>
   <si>
-    <t>자체주문번호</t>
-  </si>
-  <si>
-    <t>필수</t>
-  </si>
-  <si>
-    <t>선택</t>
-  </si>
-  <si>
-    <t>필수(중복x)</t>
-  </si>
-  <si>
-    <t>→</t>
-  </si>
-  <si>
-    <t xml:space="preserve">이 설명 부분 _x000d_
-은 삭제 후 _x000d_
-작성해 주세요.</t>
+    <t>수량</t>
+  </si>
+  <si>
+    <t>옵션</t>
+  </si>
+  <si>
+    <t>쇼핑몰주문번호 또는 자체관리번호</t>
+  </si>
+  <si>
+    <t>주문자 이름</t>
+  </si>
+  <si>
+    <t>주문자 연락처</t>
+  </si>
+  <si>
+    <t>받는분 이름</t>
+  </si>
+  <si>
+    <t>받는분 휴대폰</t>
+  </si>
+  <si>
+    <t>우편번호(선택)</t>
+  </si>
+  <si>
+    <t>전체주소</t>
+  </si>
+  <si>
+    <t>배송시 요청사항</t>
+  </si>
+  <si>
+    <t>주문수량</t>
+  </si>
+  <si>
+    <t>옵션(선택)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -75,8 +91,16 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <color rgb="FF666666"/>
+      <sz val="10"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,11 +109,16 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -97,13 +126,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,89 +484,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1"/>
+  <dimension ref="A1:L2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="40" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="11" max="11" width="8" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" ht="25" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="2" ht="20" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>